<commit_message>
A bit of a corrections to Fully Dressed
</commit_message>
<xml_diff>
--- a/System development files/FullyDressUseCases.xlsx
+++ b/System development files/FullyDressUseCases.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janis\Desktop\2.Semester Project\dmai0914-semester2-finalProject-group3\System development files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t>Use case name</t>
   </si>
@@ -60,97 +65,99 @@
     <t>The merchandise registered, customer checked in, table created, course created</t>
   </si>
   <si>
-    <t xml:space="preserve">Order was made and added to the system, notification sended to chef </t>
-  </si>
-  <si>
     <t>2.Waiter(employee)/Manager begins a new order</t>
   </si>
   <si>
-    <t>1.Customer was checked in and engaged the table. 
-Customer chooses courses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.Employee/Manager enter appropriate course or product </t>
-  </si>
-  <si>
-    <t>5.The system adds course or product to order</t>
-  </si>
-  <si>
     <t>8. Employee/Manager chooses to complete the order</t>
   </si>
   <si>
-    <t>9. The System completes the order</t>
-  </si>
-  <si>
-    <t>4a. Product is out of stock
-1.System notify that product is out of stock and cancels product adding.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Make reservation </t>
   </si>
   <si>
-    <t xml:space="preserve">Table is created </t>
-  </si>
-  <si>
     <t>The reservation is created and assigned to appropriate table.</t>
   </si>
   <si>
-    <t xml:space="preserve">1.Customer calls and specify date for reservation </t>
-  </si>
-  <si>
-    <t>2.Waiter(employee ) enters date to the system</t>
-  </si>
-  <si>
-    <t>4.Waiter(employee ) asks for additional information(name,telefon) and enter to the system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.System save information </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.System checks if there is available table that date </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.Waiter(employee) complete reservation </t>
-  </si>
-  <si>
-    <t>6.System makes reservation, assign appropriate table to that reservation and saves information.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3a. There is no free table for that day 
-1.System asks to enter another day or cancel request
+    <t>Create merchandise</t>
+  </si>
+  <si>
+    <t>Merchandise created and saved in the system</t>
+  </si>
+  <si>
+    <t>3. Manager/employee inputs information about merchandise.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.System checks if desired merchandise exists </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.Manger/empoyee complete action </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order was made and added to the system, notification sent to chef </t>
+  </si>
+  <si>
+    <t>2a. Merchandise is exists in the system</t>
+  </si>
+  <si>
+    <t>9. The System completes the order, saves it on database and sends notification to chef</t>
+  </si>
+  <si>
+    <t>Table is created and is available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Customer calls and specifys date and time for reservation </t>
+  </si>
+  <si>
+    <t>2.Waiter(employee ) enters information in the system</t>
+  </si>
+  <si>
+    <t>4. Employee/Manager inputs number of the table, where customer has been seated, in the system</t>
+  </si>
+  <si>
+    <t>5. System adds the table number to order</t>
+  </si>
+  <si>
+    <t>6.Employee/Manager inputs customers desired course or product in the system</t>
+  </si>
+  <si>
+    <t>7.The system adds course or product to order line and order line to order</t>
+  </si>
+  <si>
+    <t>8.Employee/Manager repeats the action until all desired courses or products are in the order(employee/manager repeats step 5 and 6 until all products are added)</t>
+  </si>
+  <si>
+    <t>4a. Employee enters wrong table number
+6a. Not enough ingredients for the course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2a. There are no tables available
 </t>
   </si>
   <si>
-    <t>Create merchandise</t>
-  </si>
-  <si>
-    <t>Merchandise created and saved in the system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Manager/employee creates merchandise </t>
-  </si>
-  <si>
-    <t>3. Manager/employee inputs information about merchandise.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.System checks if desired merchandise exists </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. System saves information </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.Manger/empoyee complete action </t>
-  </si>
-  <si>
-    <t>5.System creates merchandise and saves information.</t>
-  </si>
-  <si>
-    <t>2a. Merchandise is exists in the system
-1.System require create another merchandise or cancel request</t>
-  </si>
-  <si>
-    <t>6.Employee/Manager repeats the action until all desired courses or products
-are in the order(employee/manager repeats step 4 and 5 until all products are added)</t>
+    <t>4.Waiter(employee ) asks for additional information(name, telephone no.) and inputs it in the system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.Waiter(employee) completes reservation </t>
+  </si>
+  <si>
+    <t>1.Customer sits at the table and chooses courses</t>
+  </si>
+  <si>
+    <t>5.System adds the information to the reservation</t>
+  </si>
+  <si>
+    <t>3.System checks if there is available table at the desired date and adds the table to reservation</t>
+  </si>
+  <si>
+    <t>6.System creates the reservation and saves data to data base</t>
+  </si>
+  <si>
+    <t>4. System adds information to merchandise</t>
+  </si>
+  <si>
+    <t>5.System creates merchandise and saves information to data base.</t>
+  </si>
+  <si>
+    <t>1.Manager/employee begins to create a merchandise and inputs the name of it</t>
   </si>
 </sst>
 </file>
@@ -280,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -310,8 +317,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -323,7 +366,37 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -334,81 +407,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -424,9 +428,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -464,9 +468,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -501,7 +505,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -536,7 +540,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -710,16 +714,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46:C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53.85546875" customWidth="1"/>
-    <col min="2" max="2" width="57.5703125" customWidth="1"/>
+    <col min="2" max="2" width="71" customWidth="1"/>
     <col min="3" max="3" width="55.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -727,351 +731,367 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="22"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="21"/>
+      <c r="C2" s="20"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="21"/>
+      <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="21"/>
+      <c r="B4" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="20"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="20"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="26" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-    </row>
-    <row r="8" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="15" t="s">
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="32"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="33"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="29"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="22"/>
+    </row>
+    <row r="16" spans="1:3" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="41"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="29"/>
-    </row>
-    <row r="9" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="30"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="26"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="24" t="s">
+      <c r="C22" s="40"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="37"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="35"/>
+    </row>
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="23"/>
-    </row>
-    <row r="14" spans="1:3" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="C25" s="37"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+    </row>
+    <row r="33" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="32"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="22"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="21"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="36"/>
-    </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="20"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="8"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="38" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-    </row>
-    <row r="31" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="11"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="18"/>
-    </row>
-    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="20"/>
+      <c r="B33" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="18"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="20"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="B37" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="40"/>
+    </row>
+    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B38" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="21"/>
+        <v>1</v>
+      </c>
+      <c r="B38" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="37"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="36"/>
+      <c r="C39" s="37"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="37"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="4"/>
-    </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+      <c r="C41" s="4"/>
+    </row>
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B42" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C42" s="8" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="C41" s="39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="40" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
-      <c r="B43" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" s="40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
+      <c r="B43" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="B44" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="B45" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B44" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="C44" s="42"/>
+      <c r="B46" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="B44:C44"/>
+  <mergeCells count="29">
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A6:A17"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B46:C46"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A6:A15"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B18:C18"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
     <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fully dressed with added RUD merchandise
</commit_message>
<xml_diff>
--- a/System development files/FullyDressUseCases.xlsx
+++ b/System development files/FullyDressUseCases.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janis\Desktop\2.Semester Project\dmai0914-semester2-finalProject-group3\System development files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
   <si>
     <t>Use case name</t>
   </si>
@@ -158,6 +153,75 @@
   </si>
   <si>
     <t>1.Manager/employee begins to create a merchandise and inputs the name of it</t>
+  </si>
+  <si>
+    <t>Read(Find) merchandise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merchandise is found and system revealed it </t>
+  </si>
+  <si>
+    <t>1.Manager/employee send request to the system in order to find merchandise</t>
+  </si>
+  <si>
+    <t>2.System requies to input information about merchandise</t>
+  </si>
+  <si>
+    <t>4. System finds merchandise according to given information</t>
+  </si>
+  <si>
+    <t>5.System shows merchandise.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4a. Merchandise was not found 
+System asks to input another information or finish the action </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update merchandise </t>
+  </si>
+  <si>
+    <t>Merchandise is found and information was changed about it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 times a day </t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 times a day </t>
+  </si>
+  <si>
+    <t>1.Manager/employee send request to the system in order to update 
+merchandise</t>
+  </si>
+  <si>
+    <t>6.System updates merchandise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.Manager/empoyee inputs new information  in order to update it </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.Manage completes action </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.System saves information </t>
+  </si>
+  <si>
+    <t>Delete merchandise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merchandise is deleted from the system </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 times a day </t>
+  </si>
+  <si>
+    <t>1.Manager/employee send request to the system in order to delete
+merchandise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.Manager/empoyee deletes it </t>
+  </si>
+  <si>
+    <t>6.System saves changes</t>
   </si>
 </sst>
 </file>
@@ -287,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -335,6 +399,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -347,44 +468,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -392,27 +486,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -428,9 +504,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -468,9 +544,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -505,7 +581,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -540,7 +616,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -714,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46:C46"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,126 +807,126 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="19"/>
+      <c r="C1" s="38"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="39"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="20"/>
+      <c r="C3" s="39"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="20"/>
+      <c r="C4" s="39"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="20"/>
+      <c r="C5" s="39"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="27" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="21" t="s">
+      <c r="A8" s="26"/>
+      <c r="B8" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="32"/>
+      <c r="C8" s="34"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="33"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="35"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="27" t="s">
+      <c r="A10" s="26"/>
+      <c r="B10" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="32" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="29"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="31"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="23" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="28" t="s">
+      <c r="A14" s="26"/>
+      <c r="B14" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="23" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="22"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="29"/>
     </row>
     <row r="16" spans="1:3" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="9" t="s">
         <v>15</v>
       </c>
@@ -862,7 +938,7 @@
       <c r="A18" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="40" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="41"/>
@@ -871,37 +947,37 @@
       <c r="A22" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="40"/>
+      <c r="C22" s="43"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="37"/>
+      <c r="C23" s="22"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="35"/>
+      <c r="C24" s="45"/>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="37"/>
+      <c r="C25" s="22"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -950,60 +1026,60 @@
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="23" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
     </row>
     <row r="33" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="18"/>
+      <c r="C33" s="37"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="40"/>
+      <c r="C37" s="43"/>
     </row>
     <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="37"/>
+      <c r="C38" s="22"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="37"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="22"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C40" s="37"/>
+      <c r="C40" s="22"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
@@ -1056,26 +1132,313 @@
       <c r="A46" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C46" s="18"/>
+      <c r="C46" s="37"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" s="43"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="22"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" s="22"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" s="22"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" s="17"/>
+    </row>
+    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="19"/>
+      <c r="B56" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="19"/>
+      <c r="B57" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="19"/>
+      <c r="B58" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C59" s="37"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="C62" s="43"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" s="22"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C64" s="22"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C65" s="22"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C66" s="17"/>
+    </row>
+    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="19"/>
+      <c r="B68" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="19"/>
+      <c r="B69" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C69" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="19"/>
+      <c r="B70" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C70" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="19"/>
+      <c r="B71" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C71" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C72" s="37"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C76" s="43"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B77" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" s="22"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78" s="22"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C79" s="22"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B80" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C80" s="17"/>
+    </row>
+    <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B81" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C81" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="19"/>
+      <c r="B82" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C82" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="19"/>
+      <c r="B83" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C83" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="19"/>
+      <c r="B84" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C84" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C85" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A6:A17"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
+  <mergeCells count="44">
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B59:C59"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -1092,6 +1455,19 @@
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="B37:C37"/>
+    <mergeCell ref="A6:A17"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>